<commit_message>
Updates to project management
</commit_message>
<xml_diff>
--- a/Change Log.xlsx
+++ b/Change Log.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21601"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22BA8DB6-8053-47DC-B859-CAE7390C720F}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0815A22-DB71-42C8-A175-9B1B58EA195C}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-7524" yWindow="3240" windowWidth="17280" windowHeight="9900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="47">
   <si>
     <t>Team Knuth Change Log</t>
   </si>
@@ -113,6 +113,54 @@
   </si>
   <si>
     <t>added update functionality to overwrite current values in database</t>
+  </si>
+  <si>
+    <t>Added ability to load tasks to the job card</t>
+  </si>
+  <si>
+    <t>Added CSS to completed button</t>
+  </si>
+  <si>
+    <t>Reformatted the GUI</t>
+  </si>
+  <si>
+    <t>Added suspended checkbox</t>
+  </si>
+  <si>
+    <t>Added navigation menu</t>
+  </si>
+  <si>
+    <t>Created confirmation messages for when a user does an action</t>
+  </si>
+  <si>
+    <t>Added sort tasks by task urgency</t>
+  </si>
+  <si>
+    <t>Added export job card to text document</t>
+  </si>
+  <si>
+    <t>Created new Gantt chart</t>
+  </si>
+  <si>
+    <t>Updated Gantt chart</t>
+  </si>
+  <si>
+    <t>Created new gantt chart</t>
+  </si>
+  <si>
+    <t>Added new fields to Task table in the database</t>
+  </si>
+  <si>
+    <t>Updated task prioritisation</t>
+  </si>
+  <si>
+    <t>Updated progress report</t>
+  </si>
+  <si>
+    <t>completed risk assessment</t>
+  </si>
+  <si>
+    <t>Transferred buttons to navigation menu on job card</t>
   </si>
 </sst>
 </file>
@@ -537,15 +585,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B2:P57"/>
+  <dimension ref="B2:P61"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <selection activeCell="G18" sqref="G18"/>
+      <selection activeCell="B44" sqref="B44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="60.88671875" customWidth="1"/>
+    <col min="2" max="2" width="74.5546875" customWidth="1"/>
     <col min="3" max="4" width="17.44140625" customWidth="1"/>
     <col min="6" max="6" width="44.88671875" customWidth="1"/>
     <col min="7" max="8" width="17.44140625" customWidth="1"/>
@@ -878,7 +926,7 @@
     </row>
     <row r="20" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B20" s="2" t="s">
-        <v>9</v>
+        <v>44</v>
       </c>
       <c r="C20" s="2"/>
       <c r="D20" s="2"/>
@@ -894,7 +942,7 @@
     </row>
     <row r="21" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B21" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C21" s="2"/>
       <c r="D21" s="2"/>
@@ -910,7 +958,7 @@
     </row>
     <row r="22" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B22" s="2" t="s">
-        <v>26</v>
+        <v>10</v>
       </c>
       <c r="C22" s="2"/>
       <c r="D22" s="2"/>
@@ -926,7 +974,7 @@
     </row>
     <row r="23" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B23" s="2" t="s">
-        <v>27</v>
+        <v>45</v>
       </c>
       <c r="C23" s="2"/>
       <c r="D23" s="2"/>
@@ -942,7 +990,7 @@
     </row>
     <row r="24" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B24" s="2" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C24" s="2"/>
       <c r="D24" s="2"/>
@@ -958,7 +1006,7 @@
     </row>
     <row r="25" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B25" s="2" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C25" s="2"/>
       <c r="D25" s="2"/>
@@ -974,7 +1022,7 @@
     </row>
     <row r="26" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B26" s="2" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C26" s="2"/>
       <c r="D26" s="2"/>
@@ -989,7 +1037,9 @@
       <c r="P26" s="2"/>
     </row>
     <row r="27" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="B27" s="2"/>
+      <c r="B27" s="2" t="s">
+        <v>32</v>
+      </c>
       <c r="C27" s="2"/>
       <c r="D27" s="2"/>
       <c r="F27" s="2"/>
@@ -1003,7 +1053,9 @@
       <c r="P27" s="2"/>
     </row>
     <row r="28" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="B28" s="2"/>
+      <c r="B28" s="2" t="s">
+        <v>29</v>
+      </c>
       <c r="C28" s="2"/>
       <c r="D28" s="2"/>
       <c r="F28" s="2"/>
@@ -1017,7 +1069,9 @@
       <c r="P28" s="2"/>
     </row>
     <row r="29" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="B29" s="2"/>
+      <c r="B29" s="2" t="s">
+        <v>30</v>
+      </c>
       <c r="C29" s="2"/>
       <c r="D29" s="2"/>
       <c r="F29" s="2"/>
@@ -1031,7 +1085,9 @@
       <c r="P29" s="2"/>
     </row>
     <row r="30" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="B30" s="2"/>
+      <c r="B30" s="2" t="s">
+        <v>31</v>
+      </c>
       <c r="C30" s="2"/>
       <c r="D30" s="2"/>
       <c r="F30" s="2"/>
@@ -1045,7 +1101,9 @@
       <c r="P30" s="2"/>
     </row>
     <row r="31" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="B31" s="2"/>
+      <c r="B31" s="2" t="s">
+        <v>33</v>
+      </c>
       <c r="C31" s="2"/>
       <c r="D31" s="2"/>
       <c r="F31" s="2"/>
@@ -1059,7 +1117,9 @@
       <c r="P31" s="2"/>
     </row>
     <row r="32" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="B32" s="2"/>
+      <c r="B32" s="2" t="s">
+        <v>44</v>
+      </c>
       <c r="C32" s="2"/>
       <c r="D32" s="2"/>
       <c r="F32" s="2"/>
@@ -1073,7 +1133,9 @@
       <c r="P32" s="2"/>
     </row>
     <row r="33" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="B33" s="2"/>
+      <c r="B33" s="2" t="s">
+        <v>34</v>
+      </c>
       <c r="C33" s="2"/>
       <c r="D33" s="2"/>
       <c r="F33" s="2"/>
@@ -1087,7 +1149,9 @@
       <c r="P33" s="2"/>
     </row>
     <row r="34" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="B34" s="2"/>
+      <c r="B34" s="2" t="s">
+        <v>35</v>
+      </c>
       <c r="C34" s="2"/>
       <c r="D34" s="2"/>
       <c r="F34" s="2"/>
@@ -1101,7 +1165,9 @@
       <c r="P34" s="2"/>
     </row>
     <row r="35" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="B35" s="2"/>
+      <c r="B35" s="2" t="s">
+        <v>36</v>
+      </c>
       <c r="C35" s="2"/>
       <c r="D35" s="2"/>
       <c r="F35" s="2"/>
@@ -1115,7 +1181,9 @@
       <c r="P35" s="2"/>
     </row>
     <row r="36" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="B36" s="2"/>
+      <c r="B36" s="2" t="s">
+        <v>37</v>
+      </c>
       <c r="C36" s="2"/>
       <c r="D36" s="2"/>
       <c r="F36" s="2"/>
@@ -1129,7 +1197,9 @@
       <c r="P36" s="2"/>
     </row>
     <row r="37" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="B37" s="2"/>
+      <c r="B37" s="2" t="s">
+        <v>39</v>
+      </c>
       <c r="C37" s="2"/>
       <c r="D37" s="2"/>
       <c r="F37" s="2"/>
@@ -1143,7 +1213,9 @@
       <c r="P37" s="2"/>
     </row>
     <row r="38" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="B38" s="2"/>
+      <c r="B38" s="2" t="s">
+        <v>10</v>
+      </c>
       <c r="C38" s="2"/>
       <c r="D38" s="2"/>
       <c r="F38" s="2"/>
@@ -1157,7 +1229,9 @@
       <c r="P38" s="2"/>
     </row>
     <row r="39" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="B39" s="2"/>
+      <c r="B39" s="2" t="s">
+        <v>40</v>
+      </c>
       <c r="C39" s="2"/>
       <c r="D39" s="2"/>
       <c r="F39" s="2"/>
@@ -1171,7 +1245,9 @@
       <c r="P39" s="2"/>
     </row>
     <row r="40" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="B40" s="2"/>
+      <c r="B40" s="2" t="s">
+        <v>42</v>
+      </c>
       <c r="C40" s="2"/>
       <c r="D40" s="2"/>
       <c r="F40" s="2"/>
@@ -1185,7 +1261,9 @@
       <c r="P40" s="2"/>
     </row>
     <row r="41" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="B41" s="2"/>
+      <c r="B41" s="2" t="s">
+        <v>43</v>
+      </c>
       <c r="C41" s="2"/>
       <c r="D41" s="2"/>
       <c r="F41" s="2"/>
@@ -1199,7 +1277,9 @@
       <c r="P41" s="2"/>
     </row>
     <row r="42" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="B42" s="2"/>
+      <c r="B42" s="2" t="s">
+        <v>44</v>
+      </c>
       <c r="C42" s="2"/>
       <c r="D42" s="2"/>
       <c r="F42" s="2"/>
@@ -1213,7 +1293,9 @@
       <c r="P42" s="2"/>
     </row>
     <row r="43" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="B43" s="2"/>
+      <c r="B43" s="2" t="s">
+        <v>10</v>
+      </c>
       <c r="C43" s="2"/>
       <c r="D43" s="2"/>
       <c r="F43" s="2"/>
@@ -1227,7 +1309,9 @@
       <c r="P43" s="2"/>
     </row>
     <row r="44" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="B44" s="2"/>
+      <c r="B44" s="2" t="s">
+        <v>46</v>
+      </c>
       <c r="C44" s="2"/>
       <c r="D44" s="2"/>
       <c r="F44" s="2"/>
@@ -1241,7 +1325,9 @@
       <c r="P44" s="2"/>
     </row>
     <row r="45" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="B45" s="2"/>
+      <c r="B45" s="2" t="s">
+        <v>41</v>
+      </c>
       <c r="C45" s="2"/>
       <c r="D45" s="2"/>
       <c r="F45" s="2"/>
@@ -1255,7 +1341,9 @@
       <c r="P45" s="2"/>
     </row>
     <row r="46" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="B46" s="2"/>
+      <c r="B46" s="2" t="s">
+        <v>38</v>
+      </c>
       <c r="C46" s="2"/>
       <c r="D46" s="2"/>
       <c r="F46" s="2"/>
@@ -1422,6 +1510,62 @@
       <c r="O57" s="2"/>
       <c r="P57" s="2"/>
     </row>
+    <row r="58" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B58" s="2"/>
+      <c r="C58" s="2"/>
+      <c r="D58" s="2"/>
+      <c r="F58" s="2"/>
+      <c r="G58" s="2"/>
+      <c r="H58" s="2"/>
+      <c r="J58" s="2"/>
+      <c r="K58" s="2"/>
+      <c r="L58" s="2"/>
+      <c r="N58" s="2"/>
+      <c r="O58" s="2"/>
+      <c r="P58" s="2"/>
+    </row>
+    <row r="59" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B59" s="2"/>
+      <c r="C59" s="2"/>
+      <c r="D59" s="2"/>
+      <c r="F59" s="2"/>
+      <c r="G59" s="2"/>
+      <c r="H59" s="2"/>
+      <c r="J59" s="2"/>
+      <c r="K59" s="2"/>
+      <c r="L59" s="2"/>
+      <c r="N59" s="2"/>
+      <c r="O59" s="2"/>
+      <c r="P59" s="2"/>
+    </row>
+    <row r="60" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B60" s="2"/>
+      <c r="C60" s="2"/>
+      <c r="D60" s="2"/>
+      <c r="F60" s="2"/>
+      <c r="G60" s="2"/>
+      <c r="H60" s="2"/>
+      <c r="J60" s="2"/>
+      <c r="K60" s="2"/>
+      <c r="L60" s="2"/>
+      <c r="N60" s="2"/>
+      <c r="O60" s="2"/>
+      <c r="P60" s="2"/>
+    </row>
+    <row r="61" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B61" s="2"/>
+      <c r="C61" s="2"/>
+      <c r="D61" s="2"/>
+      <c r="F61" s="2"/>
+      <c r="G61" s="2"/>
+      <c r="H61" s="2"/>
+      <c r="J61" s="2"/>
+      <c r="K61" s="2"/>
+      <c r="L61" s="2"/>
+      <c r="N61" s="2"/>
+      <c r="O61" s="2"/>
+      <c r="P61" s="2"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>